<commit_message>
add member exclusion element names
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18900" yWindow="3820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="28780" yWindow="2900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>RELATION</t>
-  </si>
-  <si>
     <t>Member</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>Corporate, Non-Segment [Member]</t>
   </si>
   <si>
-    <t>Segment Reconciling Items [Member</t>
-  </si>
-  <si>
     <t>Scenario, Adjustment [Member]</t>
   </si>
   <si>
@@ -106,6 +100,60 @@
   </si>
   <si>
     <t>Reclass</t>
+  </si>
+  <si>
+    <t>Text/Label</t>
+  </si>
+  <si>
+    <t>CorporateNonSegmentMember</t>
+  </si>
+  <si>
+    <t>Element name</t>
+  </si>
+  <si>
+    <t>Segment Reconciling Items [Member]</t>
+  </si>
+  <si>
+    <t>MaterialReconcilingItemsMember</t>
+  </si>
+  <si>
+    <t>ScenarioAdjustmentMember</t>
+  </si>
+  <si>
+    <t>FairValueConcentrationOfRiskMarketRiskManagementEffectsOnIncomeOrNetAssetsMember</t>
+  </si>
+  <si>
+    <t>AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember</t>
+  </si>
+  <si>
+    <t>AccumulatedNetUnrealizedInvestmentGainLossMember</t>
+  </si>
+  <si>
+    <t>DeferredDerivativeGainLossMember</t>
+  </si>
+  <si>
+    <t>AboveMarketLeasesMember</t>
+  </si>
+  <si>
+    <t>NewAccountingPronouncementEarlyAdoptionEffectMember</t>
+  </si>
+  <si>
+    <t>Equity Components [Axis]</t>
+  </si>
+  <si>
+    <t>Legal Entity [Axis]</t>
+  </si>
+  <si>
+    <t>Parent Company [Member]</t>
+  </si>
+  <si>
+    <t>Subsidiaries [Member]</t>
+  </si>
+  <si>
+    <t>Guarantor Subsidiaries [Member]</t>
+  </si>
+  <si>
+    <t>Non-Guarantor Subsidiaries [Member]</t>
   </si>
 </sst>
 </file>
@@ -485,16 +533,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C8" sqref="C8:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -505,9 +554,11 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -533,239 +584,332 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" t="s">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>23</v>
-      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add version, release date, effective date, reformat spreadsheet
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28780" yWindow="2900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="7600" yWindow="320" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -72,9 +72,6 @@
     <t>LegalEntityAxis</t>
   </si>
   <si>
-    <t>AND</t>
-  </si>
-  <si>
     <t>ParentCompanyMember</t>
   </si>
   <si>
@@ -154,13 +151,28 @@
   </si>
   <si>
     <t>Non-Guarantor Subsidiaries [Member]</t>
+  </si>
+  <si>
+    <t>Release version</t>
+  </si>
+  <si>
+    <t>Release date</t>
+  </si>
+  <si>
+    <t>Effective date</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>AND member equals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -173,6 +185,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -193,17 +217,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,38 +585,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:E29"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -581,338 +646,557 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C2" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C3" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="4" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C4" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C6" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="7" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C7" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C8" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="G8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C9" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C10" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C11" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C12" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C13" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C14" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C15" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:29" ht="15.75" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C16" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>13</v>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C17" s="6">
+        <v>42370</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1">
-      <c r="C18" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C19" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1">
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="G19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C20" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>40</v>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C21" s="6">
+        <v>42370</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="H21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="J21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4" t="s">
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C22" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="J22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add namespace and edits to rule 15, constraints for text and element comparison to global rule logic
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="320" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="39740" yWindow="2120" windowWidth="30560" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="54">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -30,15 +35,9 @@
     <t>Member</t>
   </si>
   <si>
-    <t>Contains the text</t>
-  </si>
-  <si>
     <t>Netting</t>
   </si>
   <si>
-    <t>Equals</t>
-  </si>
-  <si>
     <t>Corporate, Non-Segment [Member]</t>
   </si>
   <si>
@@ -166,6 +165,27 @@
   </si>
   <si>
     <t>AND member equals</t>
+  </si>
+  <si>
+    <t>Member equals</t>
+  </si>
+  <si>
+    <t>Axis equals</t>
+  </si>
+  <si>
+    <t>Member element name contains the text (Case insensitive)</t>
+  </si>
+  <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>us-gaap</t>
+  </si>
+  <si>
+    <t>dei</t>
   </si>
 </sst>
 </file>
@@ -232,7 +252,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -242,6 +262,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -260,6 +281,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -585,29 +611,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC25"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="46.5" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.75" customHeight="1">
+    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -616,22 +648,26 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -649,364 +685,420 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
-    </row>
-    <row r="2" spans="1:29" ht="15.75" customHeight="1">
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+    </row>
+    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C2" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C3" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C4" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C6" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C7" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C8" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C2" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C3" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C4" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C5" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C6" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C7" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="G8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C8" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C9" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C9" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C10" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C10" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="4"/>
+      <c r="G10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C11" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C11" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C12" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C12" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C13" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C13" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C14" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C14" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C15" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C15" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:29" ht="15.75" customHeight="1">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C16" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C16" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="6">
         <v>42327</v>
@@ -1015,36 +1107,66 @@
         <v>42370</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C18" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="6">
         <v>42327</v>
@@ -1053,154 +1175,141 @@
         <v>42370</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="I19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="K19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="4" t="s">
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C20" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="F20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="K20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C20" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D20" s="4" t="s">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="6">
+        <v>42327</v>
+      </c>
+      <c r="C21" s="6">
+        <v>42370</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="I21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C21" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C22" s="6">
-        <v>42370</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add rows to v1 MemberExclusions
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellpryde/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39740" yWindow="2120" windowWidth="30560" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="12210" windowHeight="10245" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="84">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -92,9 +87,6 @@
     <t>Eliminat</t>
   </si>
   <si>
-    <t>Reconciliat</t>
-  </si>
-  <si>
     <t>Reclass</t>
   </si>
   <si>
@@ -186,13 +178,106 @@
   </si>
   <si>
     <t>dei</t>
+  </si>
+  <si>
+    <t>Reconcili</t>
+  </si>
+  <si>
+    <t>Adjustments for Change in Accounting Principle [Axis]</t>
+  </si>
+  <si>
+    <t>AdjustmentsForChangeInAccountingPrincipleAxis</t>
+  </si>
+  <si>
+    <t>Adjustments for New Accounting Pronouncements [Axis]</t>
+  </si>
+  <si>
+    <t>AdjustmentsForNewAccountingPronouncementsAxis</t>
+  </si>
+  <si>
+    <t>Change in Accounting Estimate by Type [Axis]</t>
+  </si>
+  <si>
+    <t>ChangeInAccountingEstimateByTypeAxis</t>
+  </si>
+  <si>
+    <t>Adjustments for Error Corrections [Axis]</t>
+  </si>
+  <si>
+    <t>ErrorCorrectionsAndPriorPeriodAdjustmentsRestatementByRestatementPeriodAndAmountAxis</t>
+  </si>
+  <si>
+    <t>Partner Capital Components [Axis]</t>
+  </si>
+  <si>
+    <t>PartnerCapitalComponentsAxis</t>
+  </si>
+  <si>
+    <t>Prospective Adoption of New Accounting Pronouncements [Axis]</t>
+  </si>
+  <si>
+    <t>ProspectiveAdoptionOfNewAccountingPronouncementsAxis</t>
+  </si>
+  <si>
+    <t>Nature of Error [Axis]</t>
+  </si>
+  <si>
+    <t>QuantifyingMisstatementInCurrentYearFinancialStatementsByNatureOfErrorAxis</t>
+  </si>
+  <si>
+    <t>Segments [Axis]</t>
+  </si>
+  <si>
+    <t>StatementBusinessSegmentsAxis</t>
+  </si>
+  <si>
+    <t>Other Segments [Member]</t>
+  </si>
+  <si>
+    <t>AllOtherSegmentsMember</t>
+  </si>
+  <si>
+    <t>Corporate and Other [Member]</t>
+  </si>
+  <si>
+    <t>CorporateAndOtherMember</t>
+  </si>
+  <si>
+    <t>Corporate Segment [Member]</t>
+  </si>
+  <si>
+    <t>CorporateMember</t>
+  </si>
+  <si>
+    <t>Subsidiary Issuer [Member]</t>
+  </si>
+  <si>
+    <t>SubsidiaryIssuerMember</t>
+  </si>
+  <si>
+    <t>Unallocated Financing Receivables [Member]</t>
+  </si>
+  <si>
+    <t>UnallocatedFinancingReceivablesMember</t>
+  </si>
+  <si>
+    <t>ChangeDuringPeriodFairValueDisclosureMember</t>
+  </si>
+  <si>
+    <t>CorporateAndEliminationsMember</t>
+  </si>
+  <si>
+    <t>CorporateAndReconcilingItemsMember</t>
+  </si>
+  <si>
+    <t>CorporateReconcilingItemsAndEliminationsMember</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -219,13 +304,30 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -252,7 +354,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -263,6 +365,17 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -610,36 +723,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="46.5" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" customWidth="1"/>
     <col min="6" max="6" width="46" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" customWidth="1"/>
-    <col min="10" max="10" width="31.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:31" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -648,25 +761,25 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -688,9 +801,9 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="6">
         <v>42327</v>
@@ -702,18 +815,18 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="6">
         <v>42327</v>
@@ -725,18 +838,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:31" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6">
         <v>42327</v>
@@ -748,18 +861,18 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:31" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="6">
         <v>42327</v>
@@ -771,41 +884,41 @@
         <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:31" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="6">
         <v>42327</v>
       </c>
       <c r="C6" s="6">
-        <v>42370</v>
+        <v>42417</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="6">
         <v>42327</v>
@@ -817,18 +930,18 @@
         <v>2</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="6">
         <v>42327</v>
@@ -840,25 +953,25 @@
         <v>2</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:31" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6">
         <v>42327</v>
@@ -870,25 +983,25 @@
         <v>2</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:31" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="6">
         <v>42327</v>
@@ -900,25 +1013,25 @@
         <v>2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:31" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="6">
         <v>42327</v>
@@ -930,25 +1043,25 @@
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:31" ht="15.75" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="6">
         <v>42327</v>
@@ -960,25 +1073,25 @@
         <v>2</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:31" ht="15.75" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="6">
         <v>42327</v>
@@ -990,25 +1103,25 @@
         <v>2</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:31" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="6">
         <v>42327</v>
@@ -1020,25 +1133,25 @@
         <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:31" ht="15.75" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6">
         <v>42327</v>
@@ -1050,25 +1163,25 @@
         <v>2</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:31" ht="15.75" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="6">
         <v>42327</v>
@@ -1080,25 +1193,25 @@
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="6">
         <v>42327</v>
@@ -1110,13 +1223,13 @@
         <v>12</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>13</v>
@@ -1126,9 +1239,9 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="6">
         <v>42327</v>
@@ -1140,33 +1253,33 @@
         <v>12</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="6">
         <v>42327</v>
@@ -1178,33 +1291,33 @@
         <v>12</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="6">
         <v>42327</v>
@@ -1216,33 +1329,33 @@
         <v>12</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="6">
         <v>42327</v>
@@ -1254,62 +1367,512 @@
         <v>12</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="6">
+        <v>42417</v>
+      </c>
+      <c r="C22" s="6">
+        <v>42417</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C23" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="9">
+        <v>42466</v>
+      </c>
+      <c r="C24" s="9">
+        <v>42466</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C25" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="9">
+        <v>42466</v>
+      </c>
+      <c r="C26" s="9">
+        <v>42466</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C27" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C28" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="16">
+        <v>42466</v>
+      </c>
+      <c r="C29" s="16">
+        <v>42466</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="16">
+        <v>42466</v>
+      </c>
+      <c r="C30" s="16">
+        <v>42466</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="16">
+        <v>42466</v>
+      </c>
+      <c r="C31" s="16">
+        <v>42466</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+    </row>
+    <row r="32" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="16">
+        <v>42466</v>
+      </c>
+      <c r="C32" s="16">
+        <v>42466</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L32" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="16">
+        <v>42466</v>
+      </c>
+      <c r="C33" s="16">
+        <v>42466</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+    </row>
+    <row r="34" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="16">
+        <v>42466</v>
+      </c>
+      <c r="C34" s="16">
+        <v>42466</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="16">
+        <v>42466</v>
+      </c>
+      <c r="C35" s="16">
+        <v>42466</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="16">
+        <v>42417</v>
+      </c>
+      <c r="C36" s="16">
+        <v>42417</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="16">
+        <v>42507</v>
+      </c>
+      <c r="C37" s="16">
+        <v>42507</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I37" s="14"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+    </row>
+    <row r="38" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove exclusions with reconcili and eliminat rows and appendix b
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -262,15 +262,6 @@
   </si>
   <si>
     <t>ChangeDuringPeriodFairValueDisclosureMember</t>
-  </si>
-  <si>
-    <t>CorporateAndEliminationsMember</t>
-  </si>
-  <si>
-    <t>CorporateAndReconcilingItemsMember</t>
-  </si>
-  <si>
-    <t>CorporateReconcilingItemsAndEliminationsMember</t>
   </si>
 </sst>
 </file>
@@ -287,27 +278,32 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -354,7 +350,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -369,7 +365,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -724,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="D33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1601,100 +1596,114 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="29" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="29" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="15">
         <v>42466</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C29" s="15">
         <v>42466</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="13" t="s">
+      <c r="D29" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G29" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="13" t="s">
+      <c r="G29" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="13" t="s">
+      <c r="I29" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="J29" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K29" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L29" s="13" t="s">
+      <c r="K29" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L29" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="30" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="15">
         <v>42466</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="15">
         <v>42466</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="18" t="s">
+      <c r="D30" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="17" t="s">
         <v>80</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+    </row>
+    <row r="31" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="15">
         <v>42466</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="15">
         <v>42466</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-    </row>
-    <row r="32" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="D31" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="15">
         <v>42466</v>
       </c>
-      <c r="C32" s="16">
+      <c r="C32" s="15">
         <v>42466</v>
       </c>
       <c r="D32" s="13" t="s">
@@ -1703,7 +1712,7 @@
       <c r="E32" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>68</v>
       </c>
       <c r="G32" s="13" t="s">
@@ -1716,161 +1725,84 @@
         <v>45</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K32" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="L32" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L32" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="16">
-        <v>42466</v>
-      </c>
-      <c r="C33" s="16">
-        <v>42466</v>
+      <c r="B33" s="15">
+        <v>42417</v>
+      </c>
+      <c r="C33" s="15">
+        <v>42417</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
+        <v>12</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="16">
-        <v>42466</v>
-      </c>
-      <c r="C34" s="16">
-        <v>42466</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="K34" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L34" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="16">
-        <v>42466</v>
-      </c>
-      <c r="C35" s="16">
-        <v>42466</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="16">
-        <v>42417</v>
-      </c>
-      <c r="C36" s="16">
-        <v>42417</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J36" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="K36" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L36" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="16">
+      <c r="B34" s="15">
         <v>42507</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C34" s="15">
         <v>42507</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="14" t="s">
+      <c r="D34" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F34" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H37" s="17" t="s">
+      <c r="G34" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H34" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I37" s="14"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-    </row>
-    <row r="38" spans="1:12" s="15" customFormat="1" ht="15.75" customHeight="1"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+    </row>
+    <row r="35" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
update member exclusion xlsx
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="84">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>ChangeDuringPeriodFairValueDisclosureMember</t>
+  </si>
+  <si>
+    <t>Measurement Basis [Axis]</t>
+  </si>
+  <si>
+    <t>FairValueByMeasurementBasisAxis</t>
+  </si>
+  <si>
+    <t>Changes Measurement [Member]</t>
   </si>
 </sst>
 </file>
@@ -306,9 +315,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Segoe UI"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -321,17 +330,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -363,14 +387,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -721,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="D33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1596,213 +1624,227 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="29" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
+    <row r="29" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="13">
         <v>42466</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="13">
         <v>42466</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="12" t="s">
+      <c r="G29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="I29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="J29" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="K29" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L29" s="12" t="s">
+      <c r="K29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L29" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
+    <row r="30" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="13">
         <v>42466</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="13">
         <v>42466</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="13">
+        <v>42466</v>
+      </c>
+      <c r="C31" s="13">
+        <v>42466</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-    </row>
-    <row r="31" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="15">
+      <c r="E31" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="13">
         <v>42466</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C32" s="13">
         <v>42466</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D32" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E32" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F32" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="12" t="s">
+      <c r="G32" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="I32" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="15">
-        <v>42466</v>
-      </c>
-      <c r="C32" s="15">
-        <v>42466</v>
-      </c>
-      <c r="D32" s="13" t="s">
+      <c r="J32" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="13">
+        <v>42417</v>
+      </c>
+      <c r="C33" s="13">
+        <v>42417</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="13">
+        <v>42507</v>
+      </c>
+      <c r="C34" s="13">
+        <v>42507</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="15">
-        <v>42417</v>
-      </c>
-      <c r="C33" s="15">
-        <v>42417</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L33" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="15">
-        <v>42507</v>
-      </c>
-      <c r="C34" s="15">
-        <v>42507</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H34" s="16" t="s">
+      <c r="G34" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H34" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-    </row>
-    <row r="35" spans="1:12" s="14" customFormat="1" ht="15.75" customHeight="1"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+    </row>
+    <row r="35" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
update member exclusion v1
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="0" windowWidth="12210" windowHeight="10245" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="22260" windowHeight="5175" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="86">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Changes Measurement [Member]</t>
+  </si>
+  <si>
+    <t>Partner Type [Axis]</t>
+  </si>
+  <si>
+    <t>PartnerTypeOfPartnersCapitalAccountAxis</t>
   </si>
 </sst>
 </file>
@@ -335,27 +341,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -374,31 +365,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -747,681 +745,683 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE35"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="46.42578125" customWidth="1"/>
-    <col min="6" max="6" width="46" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" style="3"/>
+    <col min="4" max="4" width="21" style="3" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46" style="3" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C2" s="5">
         <v>42370</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="A3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C3" s="5">
         <v>42370</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C4" s="5">
         <v>42370</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C5" s="5">
         <v>42370</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C6" s="5">
         <v>42417</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C7" s="5">
         <v>42370</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C8" s="5">
         <v>42370</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C9" s="5">
         <v>42370</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C10" s="6">
+      <c r="A10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C10" s="5">
         <v>42370</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C11" s="6">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C11" s="5">
         <v>42370</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C12" s="6">
+      <c r="A12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C12" s="5">
         <v>42370</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C13" s="5">
         <v>42370</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C14" s="6">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C14" s="5">
         <v>42370</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C15" s="6">
+      <c r="A15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C15" s="5">
         <v>42370</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C16" s="6">
+      <c r="A16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C16" s="5">
         <v>42370</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C17" s="6">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C17" s="5">
         <v>42370</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>35</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C18" s="6">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C18" s="5">
         <v>42370</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="4" t="s">
+      <c r="K18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C19" s="6">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C19" s="5">
         <v>42370</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L19" s="4" t="s">
+      <c r="K19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C20" s="6">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C20" s="5">
         <v>42370</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K20" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L20" s="4" t="s">
+      <c r="K20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="6">
-        <v>42327</v>
-      </c>
-      <c r="C21" s="6">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="5">
+        <v>42327</v>
+      </c>
+      <c r="C21" s="5">
         <v>42370</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="4" t="s">
+      <c r="K21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="6">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="5">
         <v>42417</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>42417</v>
       </c>
       <c r="D22" s="8" t="s">
@@ -1439,13 +1439,13 @@
       <c r="H22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="9">
@@ -1474,8 +1474,8 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="9">
@@ -1504,8 +1504,8 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A25" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="9">
@@ -1534,8 +1534,8 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="9">
@@ -1564,38 +1564,52 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="9">
-        <v>42417</v>
-      </c>
-      <c r="C27" s="9">
-        <v>42417</v>
-      </c>
-      <c r="D27" s="8" t="s">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="11">
+        <v>42466</v>
+      </c>
+      <c r="C27" s="12">
+        <v>42466</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="5" t="s">
+      <c r="F27" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A28" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="9">
@@ -1611,240 +1625,270 @@
         <v>47</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>51</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A29" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="13">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C29" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="14">
         <v>42466</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C30" s="14">
         <v>42466</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="15" t="s">
         <v>2</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L29" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="13">
-        <v>42466</v>
-      </c>
-      <c r="C30" s="13">
-        <v>42466</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>12</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="17" t="s">
-        <v>81</v>
+      <c r="F30" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="16" t="s">
-        <v>82</v>
+      <c r="H30" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J30" s="17" t="s">
-        <v>83</v>
+      <c r="J30" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="K30" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="L30" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="13">
+      <c r="L30" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="14">
         <v>42466</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="14">
         <v>42466</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>68</v>
+      <c r="F31" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="10" t="s">
-        <v>69</v>
+      <c r="H31" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J31" s="10" t="s">
+      <c r="J31" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="14">
+        <v>42466</v>
+      </c>
+      <c r="C32" s="14">
+        <v>42466</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="K31" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L31" s="11" t="s">
+      <c r="K32" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L32" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="13">
+    <row r="33" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="14">
         <v>42466</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C33" s="14">
         <v>42466</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D33" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E33" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F33" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="11" t="s">
+      <c r="G33" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I33" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="J32" s="11" t="s">
+      <c r="J33" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="K32" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L32" s="11" t="s">
+      <c r="K33" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L33" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="13">
+    <row r="34" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="14">
         <v>42417</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C34" s="14">
         <v>42417</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D34" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E34" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F34" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G34" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H34" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="I34" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="J33" s="11" t="s">
+      <c r="J34" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="K33" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L33" s="11" t="s">
+      <c r="K34" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="13">
+    <row r="35" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="14">
         <v>42507</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C35" s="14">
         <v>42507</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D35" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E35" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F35" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H34" s="14" t="s">
+      <c r="G35" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="I34" s="11"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-    </row>
-    <row r="35" spans="1:12" s="12" customFormat="1" ht="15.75" customHeight="1"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
updated exclusions xlsx plus resources files - DQC_0015
as discussed
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="82">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Corporate, Non-Segment [Member]</t>
   </si>
   <si>
-    <t>Scenario, Adjustment [Member]</t>
-  </si>
-  <si>
     <t>Fair Value, Concentration of Risk, Market Risk Management, Effects on Income or Net Assets [Member]</t>
   </si>
   <si>
@@ -97,15 +94,6 @@
   </si>
   <si>
     <t>Element name</t>
-  </si>
-  <si>
-    <t>Segment Reconciling Items [Member]</t>
-  </si>
-  <si>
-    <t>MaterialReconcilingItemsMember</t>
-  </si>
-  <si>
-    <t>ScenarioAdjustmentMember</t>
   </si>
   <si>
     <t>FairValueConcentrationOfRiskMarketRiskManagementEffectsOnIncomeOrNetAssetsMember</t>
@@ -745,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE36"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A27"/>
+      <selection activeCell="A10" activeCellId="1" sqref="A9:XFD9 A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -769,13 +757,13 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -784,25 +772,25 @@
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -826,7 +814,7 @@
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5">
         <v>42327</v>
@@ -838,18 +826,18 @@
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5">
         <v>42327</v>
@@ -861,18 +849,18 @@
         <v>2</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" s="5">
         <v>42327</v>
@@ -884,18 +872,18 @@
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5">
         <v>42327</v>
@@ -907,10 +895,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>3</v>
@@ -918,7 +906,7 @@
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" s="5">
         <v>42327</v>
@@ -930,18 +918,18 @@
         <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5">
         <v>42327</v>
@@ -953,18 +941,18 @@
         <v>2</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" s="5">
         <v>42327</v>
@@ -976,16 +964,16 @@
         <v>2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -994,7 +982,7 @@
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" s="5">
         <v>42327</v>
@@ -1006,16 +994,16 @@
         <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1024,7 +1012,7 @@
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" s="5">
         <v>42327</v>
@@ -1036,16 +1024,16 @@
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -1054,7 +1042,7 @@
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5">
         <v>42327</v>
@@ -1066,16 +1054,16 @@
         <v>2</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -1084,7 +1072,7 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="5">
         <v>42327</v>
@@ -1096,16 +1084,16 @@
         <v>2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -1114,7 +1102,7 @@
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
         <v>42327</v>
@@ -1126,16 +1114,16 @@
         <v>2</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -1144,7 +1132,7 @@
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5">
         <v>42327</v>
@@ -1156,16 +1144,16 @@
         <v>2</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -1174,7 +1162,7 @@
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5">
         <v>42327</v>
@@ -1183,19 +1171,19 @@
         <v>42370</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -1204,7 +1192,7 @@
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B16" s="5">
         <v>42327</v>
@@ -1213,28 +1201,36 @@
         <v>42370</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5">
         <v>42327</v>
@@ -1243,28 +1239,36 @@
         <v>42370</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="I17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B18" s="5">
         <v>42327</v>
@@ -1273,36 +1277,36 @@
         <v>42370</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5">
         <v>42327</v>
@@ -1311,142 +1315,126 @@
         <v>42370</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="K19" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B20" s="5">
-        <v>42327</v>
+        <v>42417</v>
       </c>
       <c r="C20" s="5">
-        <v>42370</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K20" s="6" t="s">
+        <v>42417</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="L20" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="5">
-        <v>42327</v>
-      </c>
-      <c r="C21" s="5">
-        <v>42370</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C21" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="G21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="5">
-        <v>42417</v>
-      </c>
-      <c r="C22" s="5">
-        <v>42417</v>
+        <v>40</v>
+      </c>
+      <c r="B22" s="9">
+        <v>42466</v>
+      </c>
+      <c r="C22" s="9">
+        <v>42466</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>54</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B23" s="9">
         <v>42417</v>
@@ -1455,16 +1443,16 @@
         <v>42417</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>57</v>
@@ -1476,7 +1464,7 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B24" s="9">
         <v>42466</v>
@@ -1485,16 +1473,16 @@
         <v>42466</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>59</v>
@@ -1506,58 +1494,72 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="9">
-        <v>42417</v>
-      </c>
-      <c r="C25" s="9">
-        <v>42417</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="B25" s="11">
+        <v>42466</v>
+      </c>
+      <c r="C25" s="12">
+        <v>42466</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B26" s="9">
-        <v>42466</v>
+        <v>42417</v>
       </c>
       <c r="C26" s="9">
-        <v>42466</v>
+        <v>42417</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -1566,111 +1568,113 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="11">
+        <v>40</v>
+      </c>
+      <c r="B27" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C27" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="14">
         <v>42466</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C28" s="14">
         <v>42466</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A28" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="9">
-        <v>42417</v>
-      </c>
-      <c r="C28" s="9">
-        <v>42417</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="8" t="s">
+      <c r="D28" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H28" s="8" t="s">
+      <c r="G28" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1">
+      <c r="I28" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="9">
-        <v>42417</v>
-      </c>
-      <c r="C29" s="9">
-        <v>42417</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="B29" s="14">
+        <v>42466</v>
+      </c>
+      <c r="C29" s="14">
+        <v>42466</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L29" s="19" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="30" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B30" s="14">
         <v>42466</v>
@@ -1682,33 +1686,33 @@
         <v>2</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F30" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J30" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G30" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" s="15" t="s">
+      <c r="K30" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L30" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="L30" s="15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B31" s="14">
         <v>42466</v>
@@ -1716,67 +1720,67 @@
       <c r="C31" s="14">
         <v>42466</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J31" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L31" s="19" t="s">
-        <v>80</v>
+      <c r="D31" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B32" s="14">
-        <v>42466</v>
+        <v>42417</v>
       </c>
       <c r="C32" s="14">
-        <v>42466</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>47</v>
+        <v>42417</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J32" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="K32" s="15" t="s">
-        <v>51</v>
+      <c r="K32" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="L32" s="16" t="s">
         <v>73</v>
@@ -1784,111 +1788,35 @@
     </row>
     <row r="33" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B33" s="14">
-        <v>42466</v>
+        <v>42507</v>
       </c>
       <c r="C33" s="14">
-        <v>42466</v>
+        <v>42507</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>2</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J33" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="K33" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L33" s="16" t="s">
+      <c r="G33" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="14">
-        <v>42417</v>
-      </c>
-      <c r="C34" s="14">
-        <v>42417</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L34" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A35" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="14">
-        <v>42507</v>
-      </c>
-      <c r="C35" s="14">
-        <v>42507</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-    </row>
-    <row r="36" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+    </row>
+    <row r="34" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
update exclusions .xlsx file
change member to axis for segment-related rows
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -353,7 +353,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -385,6 +385,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -735,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" activeCellId="1" sqref="A9:XFD9 A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1342,35 +1343,43 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1">
+    <row r="20" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="14">
         <v>42417</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="14">
         <v>42417</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="F20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
@@ -1389,13 +1398,13 @@
         <v>43</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1406,11 +1415,11 @@
       <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="9">
-        <v>42466</v>
-      </c>
-      <c r="C22" s="9">
-        <v>42466</v>
+      <c r="B22" s="5">
+        <v>42417</v>
+      </c>
+      <c r="C22" s="5">
+        <v>42417</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>11</v>
@@ -1419,18 +1428,18 @@
         <v>43</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
@@ -1449,13 +1458,13 @@
         <v>43</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -1467,10 +1476,10 @@
         <v>40</v>
       </c>
       <c r="B24" s="9">
-        <v>42466</v>
+        <v>42417</v>
       </c>
       <c r="C24" s="9">
-        <v>42466</v>
+        <v>42417</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>11</v>
@@ -1479,13 +1488,13 @@
         <v>43</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1496,55 +1505,41 @@
       <c r="A25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="11">
-        <v>42466</v>
-      </c>
-      <c r="C25" s="12">
-        <v>42466</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="B25" s="9">
+        <v>42417</v>
+      </c>
+      <c r="C25" s="9">
+        <v>42417</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
+      <c r="F25" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="9">
-        <v>42417</v>
+        <v>42466</v>
       </c>
       <c r="C26" s="9">
-        <v>42417</v>
+        <v>42466</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>11</v>
@@ -1553,13 +1548,13 @@
         <v>43</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -1571,10 +1566,10 @@
         <v>40</v>
       </c>
       <c r="B27" s="9">
-        <v>42417</v>
+        <v>42466</v>
       </c>
       <c r="C27" s="9">
-        <v>42417</v>
+        <v>42466</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>11</v>
@@ -1583,56 +1578,62 @@
         <v>43</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
     </row>
-    <row r="28" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="11">
         <v>42466</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="12">
         <v>42466</v>
       </c>
-      <c r="D28" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="15" t="s">
+      <c r="D28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L28" s="15" t="s">
-        <v>67</v>
-      </c>
+      <c r="F28" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="13"/>
     </row>
     <row r="29" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
@@ -1682,8 +1683,8 @@
       <c r="C30" s="14">
         <v>42466</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>2</v>
+      <c r="D30" s="21" t="s">
+        <v>11</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>43</v>
@@ -1721,7 +1722,7 @@
         <v>42466</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>43</v>
@@ -1753,37 +1754,37 @@
         <v>40</v>
       </c>
       <c r="B32" s="14">
-        <v>42417</v>
+        <v>42466</v>
       </c>
       <c r="C32" s="14">
-        <v>42417</v>
-      </c>
-      <c r="D32" s="16" t="s">
+        <v>42466</v>
+      </c>
+      <c r="D32" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="15" t="s">
         <v>43</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J32" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>73</v>
+      <c r="J32" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
update xlsx for version
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -141,9 +141,6 @@
     <t>Effective date</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>AND member equals</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>PartnerTypeOfPartnersCapitalAccountAxis</t>
+  </si>
+  <si>
+    <t>1.1.0</t>
   </si>
 </sst>
 </file>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -776,7 +776,7 @@
         <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>24</v>
@@ -788,7 +788,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>24</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5">
         <v>42327</v>
@@ -827,10 +827,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>18</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B3" s="5">
         <v>42327</v>
@@ -850,10 +850,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>19</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B4" s="5">
         <v>42327</v>
@@ -873,10 +873,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>20</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5">
         <v>42327</v>
@@ -896,10 +896,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>3</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5">
         <v>42327</v>
@@ -919,18 +919,18 @@
         <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B7" s="5">
         <v>42327</v>
@@ -942,10 +942,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>21</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B8" s="5">
         <v>42327</v>
@@ -965,13 +965,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>23</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B9" s="5">
         <v>42327</v>
@@ -995,13 +995,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>25</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B10" s="5">
         <v>42327</v>
@@ -1025,13 +1025,13 @@
         <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>26</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B11" s="5">
         <v>42327</v>
@@ -1055,13 +1055,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>27</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B12" s="5">
         <v>42327</v>
@@ -1085,13 +1085,13 @@
         <v>2</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>28</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B13" s="5">
         <v>42327</v>
@@ -1115,13 +1115,13 @@
         <v>2</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>29</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B14" s="5">
         <v>42327</v>
@@ -1145,13 +1145,13 @@
         <v>2</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>30</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B15" s="5">
         <v>42327</v>
@@ -1175,13 +1175,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>12</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B16" s="5">
         <v>42327</v>
@@ -1205,25 +1205,25 @@
         <v>11</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>33</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>14</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B17" s="5">
         <v>42327</v>
@@ -1243,25 +1243,25 @@
         <v>11</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>15</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B18" s="5">
         <v>42327</v>
@@ -1281,25 +1281,25 @@
         <v>11</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>32</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>35</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>16</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B19" s="5">
         <v>42327</v>
@@ -1319,25 +1319,25 @@
         <v>11</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>32</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>17</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="20" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B20" s="14">
         <v>42417</v>
@@ -1357,33 +1357,33 @@
         <v>11</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B21" s="9">
         <v>42417</v>
@@ -1395,16 +1395,16 @@
         <v>11</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B22" s="5">
         <v>42417</v>
@@ -1425,16 +1425,16 @@
         <v>11</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B23" s="9">
         <v>42417</v>
@@ -1455,16 +1455,16 @@
         <v>11</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B24" s="9">
         <v>42417</v>
@@ -1485,16 +1485,16 @@
         <v>11</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B25" s="9">
         <v>42417</v>
@@ -1515,16 +1515,16 @@
         <v>11</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F25" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B26" s="9">
         <v>42466</v>
@@ -1545,16 +1545,16 @@
         <v>11</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F26" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B27" s="9">
         <v>42466</v>
@@ -1575,16 +1575,16 @@
         <v>11</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>55</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B28" s="11">
         <v>42466</v>
@@ -1605,16 +1605,16 @@
         <v>11</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
@@ -1637,7 +1637,7 @@
     </row>
     <row r="29" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B29" s="14">
         <v>42466</v>
@@ -1649,33 +1649,33 @@
         <v>11</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F29" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="19" t="s">
+      <c r="I29" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J29" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>79</v>
-      </c>
       <c r="K29" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B30" s="14">
         <v>42466</v>
@@ -1687,33 +1687,33 @@
         <v>11</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G30" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>65</v>
-      </c>
       <c r="I30" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J30" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L30" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B31" s="14">
         <v>42466</v>
@@ -1725,33 +1725,33 @@
         <v>11</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>65</v>
-      </c>
       <c r="I31" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J31" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L31" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L31" s="16" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:26" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B32" s="14">
         <v>42466</v>
@@ -1763,33 +1763,33 @@
         <v>11</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H32" s="15" t="s">
+      <c r="I32" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="I32" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32" s="15" t="s">
+      <c r="K32" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32" s="15" t="s">
         <v>66</v>
-      </c>
-      <c r="K32" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L32" s="15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B33" s="14">
         <v>42507</v>
@@ -1801,16 +1801,16 @@
         <v>2</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="15"/>

</xml_diff>

<commit_message>
update dqc_0015 exclusion.xlsx and docs/readme
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="85">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>Initial Release</t>
+  </si>
+  <si>
+    <t>3.6.0</t>
+  </si>
+  <si>
+    <t>ConsolidatedEntities [Axis]</t>
+  </si>
+  <si>
+    <t>ConsolidatedEntitiesAxis</t>
   </si>
 </sst>
 </file>
@@ -371,7 +380,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -412,6 +421,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -760,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE34"/>
+  <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1869,6 +1882,181 @@
         <v>63</v>
       </c>
     </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A35" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="4">
+        <v>42894</v>
+      </c>
+      <c r="C35" s="4">
+        <v>42894</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="I35" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A36" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="4">
+        <v>42894</v>
+      </c>
+      <c r="C36" s="4">
+        <v>42894</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="I36" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A37" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="4">
+        <v>42894</v>
+      </c>
+      <c r="C37" s="4">
+        <v>42894</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="I37" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A38" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="4">
+        <v>42894</v>
+      </c>
+      <c r="C38" s="4">
+        <v>42894</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="I38" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A39" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="4">
+        <v>42894</v>
+      </c>
+      <c r="C39" s="4">
+        <v>42894</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
v6 updated member exclusion .xlsx file
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="87">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>Consolidated Entities [Axis]</t>
+  </si>
+  <si>
+    <t>Difference between Revenue Guidance in Effect before and after Topic 606 [Member]</t>
+  </si>
+  <si>
+    <t>DifferenceBetweenRevenueGuidanceInEffectBeforeAndAfterTopic606Member</t>
   </si>
 </sst>
 </file>
@@ -756,9 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE39"/>
+  <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -2053,6 +2061,32 @@
         <v>71</v>
       </c>
     </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A40" s="3">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4">
+        <v>43235</v>
+      </c>
+      <c r="C40" s="4">
+        <v>43235</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Public Exposure v6 updates for DQC approval (#309)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="87">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>Consolidated Entities [Axis]</t>
+  </si>
+  <si>
+    <t>Difference between Revenue Guidance in Effect before and after Topic 606 [Member]</t>
+  </si>
+  <si>
+    <t>DifferenceBetweenRevenueGuidanceInEffectBeforeAndAfterTopic606Member</t>
   </si>
 </sst>
 </file>
@@ -756,9 +762,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE39"/>
+  <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -2053,6 +2061,32 @@
         <v>71</v>
       </c>
     </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A40" s="3">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4">
+        <v>43235</v>
+      </c>
+      <c r="C40" s="4">
+        <v>43235</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Merge for v14.01. (#527)
* Update DQC_0015_MemberExclusions.xlsx

* Updated namespace for 2021 version of the taxonomy for SEC changes

* Update DQC_0104.md

* Update rulesetMap.json

gaap_2021_support

* Remove incorrectly named GAAP 2021 file

gaap_2021_support

* Add correctly named GAAP 2021 file

* Updated rule 48 to single error for multiple Calc Networks

* Updated rules for changes to Rule 48

Also updated Rule 43 for net income item excluded.

* Updated rule set 14 for changes to rule 48

* Updated Rule 99 for SHE exceptions.

* Updated Version 14 for V14.0.1

* Update documentation - dqc_0001 list of axes .xlsx

* Remove v14 rulesets for reload as V14.zip

* Reload v14.0.1 rulesets as V14.zip

* Update rulesetMap.json

Co-authored-by: campbellpryde 
Co-authored-by: Derek Gengenbacher
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
+++ b/docs/DQC_US_0015/DQC_0015_MemberExclusions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DJT\Documents\GitHub\DQC\dqc_us_rules\docs\DQC_US_0015\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4984591-48CA-41E3-93B8-2E8AE28A1FFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="22260" windowHeight="5175" tabRatio="500"/>
+    <workbookView xWindow="2055" yWindow="1380" windowWidth="24060" windowHeight="12255" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="88">
   <si>
     <t>Dimensionality</t>
   </si>
@@ -280,16 +286,19 @@
   </si>
   <si>
     <t>DifferenceBetweenRevenueGuidanceInEffectBeforeAndAfterTopic606Member</t>
+  </si>
+  <si>
+    <t>basisswap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -371,7 +380,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -414,6 +423,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -435,6 +453,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -761,14 +782,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
     <col min="2" max="3" width="14.42578125" style="3"/>
@@ -784,7 +805,7 @@
     <col min="13" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.75" customHeight="1">
+    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
@@ -841,7 +862,7 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
     </row>
-    <row r="2" spans="1:31" ht="15.75" customHeight="1">
+    <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -864,7 +885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.75" customHeight="1">
+    <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -887,7 +908,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15.75" customHeight="1">
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>1</v>
       </c>
@@ -910,7 +931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="15.75" customHeight="1">
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>1</v>
       </c>
@@ -933,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="15.75" customHeight="1">
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>80</v>
       </c>
@@ -956,7 +977,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="15.75" customHeight="1">
+    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21">
         <v>1</v>
       </c>
@@ -979,37 +1000,49 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A8" s="21">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4">
-        <v>42327</v>
-      </c>
-      <c r="C8" s="4">
-        <v>42370</v>
-      </c>
-      <c r="D8" s="5" t="s">
+    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
+        <v>14</v>
+      </c>
+      <c r="B8" s="29">
+        <v>44195</v>
+      </c>
+      <c r="C8" s="29">
+        <v>44195</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:31" ht="15.75" customHeight="1">
+      <c r="E8" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+    </row>
+    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21">
         <v>1</v>
       </c>
@@ -1026,20 +1059,20 @@
         <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:31" ht="15.75" customHeight="1">
+    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21">
         <v>1</v>
       </c>
@@ -1056,20 +1089,20 @@
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:31" ht="15.75" customHeight="1">
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
         <v>1</v>
       </c>
@@ -1086,20 +1119,20 @@
         <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:31" ht="15.75" customHeight="1">
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
         <v>1</v>
       </c>
@@ -1116,20 +1149,20 @@
         <v>40</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:31" ht="15.75" customHeight="1">
+    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21">
         <v>1</v>
       </c>
@@ -1146,20 +1179,20 @@
         <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:31" ht="15.75" customHeight="1">
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21">
         <v>1</v>
       </c>
@@ -1176,20 +1209,20 @@
         <v>40</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:31" ht="15.75" customHeight="1">
+    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
         <v>1</v>
       </c>
@@ -1200,26 +1233,26 @@
         <v>42370</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:31" ht="15.75" customHeight="1">
+    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
         <v>1</v>
       </c>
@@ -1236,28 +1269,20 @@
         <v>41</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>46</v>
+        <v>31</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1">
+        <v>12</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21">
         <v>1</v>
       </c>
@@ -1286,16 +1311,16 @@
         <v>39</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>45</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21">
         <v>1</v>
       </c>
@@ -1324,16 +1349,16 @@
         <v>39</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>45</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21">
         <v>1</v>
       </c>
@@ -1362,91 +1387,99 @@
         <v>39</v>
       </c>
       <c r="J19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4">
+        <v>42327</v>
+      </c>
+      <c r="C20" s="4">
+        <v>42370</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" s="5" t="s">
+      <c r="K20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A20" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="13">
-        <v>42417</v>
-      </c>
-      <c r="C20" s="13">
-        <v>42417</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1">
+    <row r="21" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="13">
         <v>42417</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="13">
         <v>42417</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1">
+      <c r="D21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="8">
         <v>42417</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="8">
         <v>42417</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -1456,27 +1489,27 @@
         <v>41</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1">
+        <v>55</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="4">
         <v>42417</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="4">
         <v>42417</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -1486,20 +1519,20 @@
         <v>41</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1">
+        <v>49</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>80</v>
       </c>
@@ -1516,20 +1549,20 @@
         <v>41</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>80</v>
       </c>
@@ -1546,28 +1579,28 @@
         <v>41</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B26" s="8">
-        <v>42466</v>
+        <v>42417</v>
       </c>
       <c r="C26" s="8">
-        <v>42466</v>
+        <v>42417</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>11</v>
@@ -1576,20 +1609,20 @@
         <v>41</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>80</v>
       </c>
@@ -1606,71 +1639,57 @@
         <v>41</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>45</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="8">
         <v>42466</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="8">
         <v>42466</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="12"/>
-      <c r="W28" s="12"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
-    </row>
-    <row r="29" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1">
+      <c r="D28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="10">
         <v>42466</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="11">
         <v>42466</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -1679,29 +1698,35 @@
       <c r="E29" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="17" t="s">
-        <v>75</v>
+      <c r="F29" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L29" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1">
+      <c r="H29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+    </row>
+    <row r="30" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>80</v>
       </c>
@@ -1711,35 +1736,35 @@
       <c r="C30" s="13">
         <v>42466</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="14" t="s">
+      <c r="D30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="J30" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="L30" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1">
+      <c r="J30" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L30" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>80</v>
       </c>
@@ -1749,35 +1774,35 @@
       <c r="C31" s="13">
         <v>42466</v>
       </c>
-      <c r="D31" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="15" t="s">
+      <c r="D31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F31" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" s="15" t="s">
+      <c r="G31" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="K31" s="15" t="s">
+      <c r="J31" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" s="14" t="s">
         <v>45</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>80</v>
       </c>
@@ -1787,129 +1812,129 @@
       <c r="C32" s="13">
         <v>42466</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="14" t="s">
+      <c r="D32" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F32" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32" s="14" t="s">
+      <c r="G32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J32" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="L32" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="16" customFormat="1" ht="15.75" customHeight="1">
+      <c r="J32" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>80</v>
       </c>
       <c r="B33" s="13">
+        <v>42466</v>
+      </c>
+      <c r="C33" s="13">
+        <v>42466</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="13">
         <v>42507</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C34" s="13">
         <v>42507</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D34" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E34" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F34" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G33" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="19" t="s">
+      <c r="G34" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="I33" s="15"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-    </row>
-    <row r="34" spans="1:12" s="16" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="25">
+      <c r="I34" s="15"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+    </row>
+    <row r="35" spans="1:12" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="25">
         <v>2</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B35" s="23">
         <v>42642</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C35" s="26">
         <v>42736</v>
       </c>
-      <c r="D34" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="9" t="s">
+      <c r="D35" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H34" s="9" t="s">
+      <c r="G35" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A35" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="11">
-        <v>42894</v>
-      </c>
-      <c r="C35" s="11">
-        <v>42894</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L35" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
         <v>82</v>
       </c>
@@ -1938,16 +1963,16 @@
         <v>39</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>45</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
         <v>82</v>
       </c>
@@ -1976,16 +2001,16 @@
         <v>39</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>45</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="27" t="s">
         <v>82</v>
       </c>
@@ -2014,16 +2039,16 @@
         <v>39</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>45</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="27" t="s">
         <v>82</v>
       </c>
@@ -2052,38 +2077,76 @@
         <v>39</v>
       </c>
       <c r="J39" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="11">
+        <v>42894</v>
+      </c>
+      <c r="C40" s="11">
+        <v>42894</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J40" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="K39" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L39" s="9" t="s">
+      <c r="K40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L40" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A40" s="3">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
         <v>6</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B41" s="4">
         <v>43235</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C41" s="4">
         <v>43235</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H40" s="3" t="s">
+      <c r="G41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>